<commit_message>
nouveau cahier des charges pour revue
</commit_message>
<xml_diff>
--- a/Gestion/Mega_planif.xlsx
+++ b/Gestion/Mega_planif.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="231">
   <si>
     <t>Objectif</t>
   </si>
@@ -703,9 +703,6 @@
     <t>3.T.7.2</t>
   </si>
   <si>
-    <t>3.T.7.3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Facilité des connections </t>
   </si>
   <si>
@@ -719,6 +716,9 @@
   </si>
   <si>
     <t>+/- 2 actions</t>
+  </si>
+  <si>
+    <t>À déterminer</t>
   </si>
 </sst>
 </file>
@@ -1243,13 +1243,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z510"/>
+  <dimension ref="A1:Z509"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" ySplit="4" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="I101" sqref="I101"/>
+      <selection pane="bottomRight" activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2433,7 +2433,9 @@
       <c r="E35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
@@ -2464,7 +2466,9 @@
       <c r="E36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -2495,7 +2499,9 @@
       <c r="E37" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -2526,7 +2532,9 @@
       <c r="E38" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F38" s="2"/>
+      <c r="F38" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -2588,7 +2596,9 @@
       <c r="E40" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -2619,7 +2629,9 @@
       <c r="E41" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
@@ -2650,7 +2662,9 @@
       <c r="E42" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
@@ -2681,7 +2695,9 @@
       <c r="E43" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F43" s="2"/>
+      <c r="F43" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
@@ -2749,7 +2765,9 @@
       <c r="E45" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F45" s="2"/>
+      <c r="F45" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
@@ -3420,10 +3438,10 @@
         <v>160</v>
       </c>
       <c r="F64" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G64" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>230</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>67</v>
@@ -3457,7 +3475,9 @@
       <c r="E65" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="F65" s="2"/>
+      <c r="F65" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -3733,13 +3753,13 @@
         <v>166</v>
       </c>
       <c r="E73" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F73" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="F73" s="16" t="s">
+      <c r="G73" s="16" t="s">
         <v>227</v>
-      </c>
-      <c r="G73" s="16" t="s">
-        <v>228</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>36</v>
@@ -3874,7 +3894,9 @@
       <c r="E77" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="F77" s="2"/>
+      <c r="F77" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -3936,7 +3958,9 @@
       <c r="E79" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F79" s="2"/>
+      <c r="F79" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -3967,7 +3991,9 @@
       <c r="E80" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F80" s="2"/>
+      <c r="F80" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -3998,7 +4024,9 @@
       <c r="E81" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F81" s="2"/>
+      <c r="F81" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -4193,15 +4221,18 @@
       <c r="Y86" s="2"/>
       <c r="Z86" s="2"/>
     </row>
-    <row r="87" spans="1:26" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B87" s="2"/>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A87" s="3"/>
+      <c r="B87" s="2" t="s">
+        <v>126</v>
+      </c>
       <c r="C87" s="2"/>
-      <c r="D87" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="F87" s="2"/>
-      <c r="G87" s="4"/>
+      <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
@@ -4224,13 +4255,13 @@
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="3"/>
-      <c r="B88" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="D88" s="2"/>
       <c r="E88" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -4257,20 +4288,27 @@
     <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="3"/>
       <c r="B89" s="2"/>
-      <c r="C89" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="E89" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
+      <c r="J89" s="2">
+        <v>2</v>
+      </c>
+      <c r="K89" s="2">
+        <v>4</v>
+      </c>
+      <c r="L89" s="2">
+        <f>K89*J89</f>
+        <v>8</v>
+      </c>
       <c r="M89" s="2"/>
       <c r="N89" s="2"/>
       <c r="O89" s="2"/>
@@ -4291,10 +4329,10 @@
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -4304,11 +4342,11 @@
         <v>2</v>
       </c>
       <c r="K90" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L90" s="2">
-        <f>K90*J90</f>
-        <v>8</v>
+        <f t="shared" ref="L90:L91" si="6">K90*J90</f>
+        <v>2</v>
       </c>
       <c r="M90" s="2"/>
       <c r="N90" s="2"/>
@@ -4330,10 +4368,10 @@
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -4346,7 +4384,7 @@
         <v>1</v>
       </c>
       <c r="L91" s="2">
-        <f t="shared" ref="L91:L92" si="6">K91*J91</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="M91" s="2"/>
@@ -4367,27 +4405,20 @@
     <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="3"/>
       <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="C92" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D92" s="2"/>
       <c r="E92" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
-      <c r="J92" s="2">
-        <v>2</v>
-      </c>
-      <c r="K92" s="2">
-        <v>1</v>
-      </c>
-      <c r="L92" s="2">
-        <f t="shared" si="6"/>
-        <v>2</v>
-      </c>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
+      <c r="L92" s="2"/>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -4406,20 +4437,27 @@
     <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="3"/>
       <c r="B93" s="2"/>
-      <c r="C93" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="E93" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
-      <c r="L93" s="2"/>
+      <c r="J93" s="2">
+        <v>2</v>
+      </c>
+      <c r="K93" s="2">
+        <v>3</v>
+      </c>
+      <c r="L93" s="2">
+        <f>K93*J93</f>
+        <v>6</v>
+      </c>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="2"/>
@@ -4440,10 +4478,10 @@
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -4453,11 +4491,11 @@
         <v>2</v>
       </c>
       <c r="K94" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L94" s="2">
-        <f>K94*J94</f>
-        <v>6</v>
+        <f t="shared" ref="L94:L95" si="7">K94*J94</f>
+        <v>20</v>
       </c>
       <c r="M94" s="2"/>
       <c r="N94" s="2"/>
@@ -4479,10 +4517,10 @@
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -4492,11 +4530,11 @@
         <v>2</v>
       </c>
       <c r="K95" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L95" s="2">
-        <f t="shared" ref="L95:L96" si="7">K95*J95</f>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>4</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
@@ -4516,27 +4554,20 @@
     <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A96" s="3"/>
       <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="C96" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D96" s="2"/>
       <c r="E96" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
-      <c r="J96" s="2">
-        <v>2</v>
-      </c>
-      <c r="K96" s="2">
-        <v>2</v>
-      </c>
-      <c r="L96" s="2">
-        <f t="shared" si="7"/>
-        <v>4</v>
-      </c>
+      <c r="J96" s="2"/>
+      <c r="K96" s="2"/>
+      <c r="L96" s="2"/>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
       <c r="O96" s="2"/>
@@ -4555,20 +4586,27 @@
     <row r="97" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A97" s="3"/>
       <c r="B97" s="2"/>
-      <c r="C97" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2" t="s">
+        <v>136</v>
+      </c>
       <c r="E97" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
-      <c r="J97" s="2"/>
-      <c r="K97" s="2"/>
-      <c r="L97" s="2"/>
+      <c r="J97" s="2">
+        <v>2</v>
+      </c>
+      <c r="K97" s="2">
+        <v>3</v>
+      </c>
+      <c r="L97" s="2">
+        <f>K97*J97</f>
+        <v>6</v>
+      </c>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
       <c r="O97" s="2"/>
@@ -4589,10 +4627,10 @@
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
       <c r="D98" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -4602,11 +4640,11 @@
         <v>2</v>
       </c>
       <c r="K98" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L98" s="2">
-        <f>K98*J98</f>
-        <v>6</v>
+        <f t="shared" ref="L98:L99" si="8">K98*J98</f>
+        <v>12</v>
       </c>
       <c r="M98" s="2"/>
       <c r="N98" s="2"/>
@@ -4628,10 +4666,10 @@
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
       <c r="D99" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -4641,11 +4679,11 @@
         <v>2</v>
       </c>
       <c r="K99" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L99" s="2">
-        <f t="shared" ref="L99:L100" si="8">K99*J99</f>
-        <v>12</v>
+        <f t="shared" si="8"/>
+        <v>8</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -4663,29 +4701,17 @@
       <c r="Z99" s="2"/>
     </row>
     <row r="100" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A100" s="3"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E100" s="5" t="s">
-        <v>94</v>
-      </c>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
-      <c r="J100" s="2">
-        <v>2</v>
-      </c>
-      <c r="K100" s="2">
-        <v>4</v>
-      </c>
-      <c r="L100" s="2">
-        <f t="shared" si="8"/>
-        <v>8</v>
-      </c>
+      <c r="J100" s="2"/>
+      <c r="K100" s="2"/>
+      <c r="L100" s="2"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -15743,33 +15769,6 @@
       <c r="X509" s="2"/>
       <c r="Y509" s="2"/>
       <c r="Z509" s="2"/>
-    </row>
-    <row r="510" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="B510" s="2"/>
-      <c r="C510" s="2"/>
-      <c r="D510" s="2"/>
-      <c r="E510" s="2"/>
-      <c r="F510" s="2"/>
-      <c r="G510" s="2"/>
-      <c r="H510" s="2"/>
-      <c r="I510" s="2"/>
-      <c r="J510" s="2"/>
-      <c r="K510" s="2"/>
-      <c r="L510" s="2"/>
-      <c r="M510" s="2"/>
-      <c r="N510" s="2"/>
-      <c r="O510" s="2"/>
-      <c r="P510" s="2"/>
-      <c r="Q510" s="2"/>
-      <c r="R510" s="2"/>
-      <c r="S510" s="2"/>
-      <c r="T510" s="2"/>
-      <c r="U510" s="2"/>
-      <c r="V510" s="2"/>
-      <c r="W510" s="2"/>
-      <c r="X510" s="2"/>
-      <c r="Y510" s="2"/>
-      <c r="Z510" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>